<commit_message>
Current Follow-up and Baseline
</commit_message>
<xml_diff>
--- a/Data/Baseline.xlsx
+++ b/Data/Baseline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akunerth/Dropbox (University of Oregon)/Rapid Response Research (R3)/Data Management R3/EE_R3 Question Bank/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7B18AF3-F9BD-6646-8EB4-20780A0703B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{550DD72F-6120-754E-9654-9E2EF3B1B4C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3580" yWindow="960" windowWidth="27080" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5520" yWindow="1600" windowWidth="27080" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="138">
   <si>
     <t xml:space="preserve">• Not at all _x000D_
 • Several days _x000D_
@@ -68,18 +68,6 @@
 • Sometimes 
 • Usually  
 • Always </t>
-  </si>
-  <si>
-    <t>Do you currently have access to free food for your household? Examples of free food include food pantries and programs, SNAP etc.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">• Yes I have access to free food resources 
-• No, but I know where/how I can access free food resources  
-• No, I am not eligible for free food resources  
-• Unsure </t>
-  </si>
-  <si>
-    <t>Meet Basic Needs for Health and Well-Being</t>
   </si>
   <si>
     <t xml:space="preserve">What is the zip code for your current residence? </t>
@@ -1010,10 +998,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D81"/>
+  <dimension ref="A1:D80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74:XFD80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1025,455 +1013,455 @@
   <sheetData>
     <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D1" t="s">
         <v>137</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="D1" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="96" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="144" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="128" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="96" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="192" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="128" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="96" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="160" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="96" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="80" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="128" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="224" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="240" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="112" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="112" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="224" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="112" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="96" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="80" x14ac:dyDescent="0.2">
@@ -1484,18 +1472,18 @@
         <v>2</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="80" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="80" x14ac:dyDescent="0.2">
@@ -1506,40 +1494,40 @@
         <v>4</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="80" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="80" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="80" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="80" x14ac:dyDescent="0.2">
@@ -1550,29 +1538,29 @@
         <v>4</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="80" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="80" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="80" x14ac:dyDescent="0.2">
@@ -1583,311 +1571,300 @@
         <v>8</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="80" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="96" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="80" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B57" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C57" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="144" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="96" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="80" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C70" s="2" t="s">
         <v>125</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C73" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C74" s="1" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="64" x14ac:dyDescent="0.2">
-      <c r="A74" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C75" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A76" s="1" t="s">
+      <c r="B76" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B76" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A77" s="1" t="s">
-        <v>132</v>
-      </c>
       <c r="B77" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>131</v>
+        <v>70</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A81" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Baseline updated with sources.
</commit_message>
<xml_diff>
--- a/Data/Baseline.xlsx
+++ b/Data/Baseline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akunerth/Dropbox (University of Oregon)/Rapid Response Research (R3)/Data Management R3/EE_R3 Question Bank/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{550DD72F-6120-754E-9654-9E2EF3B1B4C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47619FC1-4124-4146-8035-5AB249994592}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5520" yWindow="1600" windowWidth="27080" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="20600" windowHeight="15580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="166">
   <si>
     <t xml:space="preserve">• Not at all _x000D_
 • Several days _x000D_
@@ -197,9 +197,6 @@
   </si>
   <si>
     <t>Single select from 1-20 children, then &gt; 20</t>
-  </si>
-  <si>
-    <t>Include all children, teenagers, adults, and yourself.</t>
   </si>
   <si>
     <t xml:space="preserve">What is your race? Select all that apply 
@@ -406,10 +403,6 @@
 [Asked of all children]</t>
   </si>
   <si>
-    <t>The next set of questinos are related to your experience with the COVID-19 virus.
-Instructions: Please answer each quesstion to the best of your ability. All questions are optional. Coronavirus is also known as COVID-19, and refers to the global pandemic occurring in late 2019 and throughout 2020</t>
-  </si>
-  <si>
     <t>Have you been suspected or diagnosed with coronavirus (COVID-19)?</t>
   </si>
   <si>
@@ -532,10 +525,6 @@
   </si>
   <si>
     <t>Financial Strain</t>
-  </si>
-  <si>
-    <t>[If very hard, hard or somewhat hard to pay for basics]
-Which of these needs have been hard to pay for in the past moth? Select all that apply</t>
   </si>
   <si>
     <t>•  Food
@@ -642,15 +631,121 @@
   <si>
     <t>Source</t>
   </si>
+  <si>
+    <t>U.S. Census</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RAPID Team Modified from U.S. Census </t>
+  </si>
+  <si>
+    <t>Link (as available)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RAPID Team Modified from U.S. Census 
+</t>
+  </si>
+  <si>
+    <t>https://www.census.gov/data/tables/time-series/demo/families/children.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U.S. Census
+</t>
+  </si>
+  <si>
+    <t>https://www.census.gov/acs/www/about/why-we-ask-each-question/sex/?sec_ak_reference=18.28e8d93f.1590627222.663bae5</t>
+  </si>
+  <si>
+    <t>https://www.census.gov/acs/www/about/why-we-ask-each-question/citizenship/</t>
+  </si>
+  <si>
+    <t>How many people currently live in your home?
+Include all children, teenagers, adults, and yourself.</t>
+  </si>
+  <si>
+    <t>https://www.pewresearch.org/hispanic/2004/03/19/generational-differences/</t>
+  </si>
+  <si>
+    <t>RAPID Team Modified from Pew Study</t>
+  </si>
+  <si>
+    <t>https://www.census2020now.org/faces-blog/same-sex-households-2020-census-r3976</t>
+  </si>
+  <si>
+    <t>https://www.census.gov/acs/www/about/why-we-ask-each-question/language/</t>
+  </si>
+  <si>
+    <t>RAPID Team Modified</t>
+  </si>
+  <si>
+    <t>https://adata.org/faq/what-definition-disability-under-ada#:~:text=The%20ADA%20defines%20a%20person,not%20currently%20have%20a%20disability.</t>
+  </si>
+  <si>
+    <t>RAPID Team Modified. From U.S. Census and ADA</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov/nchs/nhis/health_insurance/hi_content.htm</t>
+  </si>
+  <si>
+    <t>RAPID Team Modified from NHIS</t>
+  </si>
+  <si>
+    <t>Developed by RAPID Team</t>
+  </si>
+  <si>
+    <t>GAD-2</t>
+  </si>
+  <si>
+    <t>PHQ-2</t>
+  </si>
+  <si>
+    <t>The next set of questions are related to your experience with the COVID-19 virus.
+Instructions: Please answer each quesstion to the best of your ability. All questions are optional. Coronavirus is also known as COVID-19, and refers to the global pandemic occurring in late 2019 and throughout 2020</t>
+  </si>
+  <si>
+    <t>https://www.jstor.org/stable/pdf/40967322.pdf?casa_token=8BWrXEu4O5QAAAAA:v8l4I7NHebQhvvF9b3K6MeP2aY_Xf8VjkTWWTVui01iBUeyvscZB_ZVwMHB64Ioj05dyOmqzjTgI3OgJ7Hmz7uoXrbpAV6hT_9r6-a45miUEoP5vQSA</t>
+  </si>
+  <si>
+    <t>RAPID Team Modified from single item Stress measure</t>
+  </si>
+  <si>
+    <t>PSOC</t>
+  </si>
+  <si>
+    <t>https://www.census.gov/acs/www/about/why-we-ask-each-question/income/#:~:text=We%20ask%20questions%20about%20the,assistance%20for%20populations%20in%20need.</t>
+  </si>
+  <si>
+    <t>RAPID Team Modified from Economic Harship Questionnaire</t>
+  </si>
+  <si>
+    <t>NIH Toolbox Item Bank v2.0</t>
+  </si>
+  <si>
+    <t>IOM Financial Strain</t>
+  </si>
+  <si>
+    <t>[If very hard, hard or somewhat hard to pay for basics]
+Which of these needs have been hard to pay for in the past month? Select all that apply</t>
+  </si>
+  <si>
+    <t>CBCL</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -673,10 +768,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -684,8 +780,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -998,10 +1098,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D80"/>
+  <dimension ref="A1:E80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="A74" sqref="A74:XFD80"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D80" sqref="D80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1009,23 +1109,28 @@
     <col min="1" max="1" width="54.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="51.83203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="27.5" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" s="1" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -1035,8 +1140,11 @@
       <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="D2" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -1046,8 +1154,11 @@
       <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="96" x14ac:dyDescent="0.2">
+      <c r="D3" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="144" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>34</v>
       </c>
@@ -1057,8 +1168,14 @@
       <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="D4" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -1068,8 +1185,11 @@
       <c r="C5" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="144" x14ac:dyDescent="0.2">
+      <c r="D5" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="144" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -1079,10 +1199,13 @@
       <c r="C6" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="D6" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="64" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>36</v>
+        <v>143</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>35</v>
@@ -1090,8 +1213,11 @@
       <c r="C7" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="D7" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="240" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -1101,8 +1227,14 @@
       <c r="C8" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="D8" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="160" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
@@ -1112,8 +1244,14 @@
       <c r="C9" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="128" x14ac:dyDescent="0.2">
+      <c r="D9" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="144" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
@@ -1123,8 +1261,14 @@
       <c r="C10" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+      <c r="D10" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="176" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>22</v>
       </c>
@@ -1134,10 +1278,16 @@
       <c r="C11" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="96" x14ac:dyDescent="0.2">
+      <c r="D11" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="96" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>24</v>
@@ -1145,8 +1295,11 @@
       <c r="C12" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="192" x14ac:dyDescent="0.2">
+      <c r="D12" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="192" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>25</v>
       </c>
@@ -1156,8 +1309,14 @@
       <c r="C13" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="D13" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="64" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
@@ -1167,8 +1326,11 @@
       <c r="C14" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="D14" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="64" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>29</v>
       </c>
@@ -1178,10 +1340,13 @@
       <c r="C15" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="128" x14ac:dyDescent="0.2">
+      <c r="D15" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="256" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>31</v>
@@ -1189,282 +1354,370 @@
       <c r="C16" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="64" x14ac:dyDescent="0.2">
+      <c r="D16" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="64" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="96" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="48" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B18" s="1" t="s">
+      <c r="C20" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="48" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B19" s="1" t="s">
+      <c r="D20" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="160" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="96" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="160" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
+      <c r="D21" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="96" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="96" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
+      <c r="C22" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="80" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="80" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+      <c r="C23" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="128" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="128" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="C24" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
+      <c r="C25" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C25" s="2" t="s">
+    </row>
+    <row r="26" spans="1:5" ht="112" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="48" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
+      <c r="B26" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="C26" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="224" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="224" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="C27" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="112" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="48" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="C28" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="240" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="240" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="C29" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="112" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="112" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="C30" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E30" s="3"/>
+    </row>
+    <row r="31" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="48" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="C31" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="112" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="112" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
+      <c r="C32" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="224" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="112" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="96" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="224" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="64" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="64" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="112" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
+      <c r="B37" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C37" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="96" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="48" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="64" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
-        <v>80</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="64" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="64" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="64" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="64" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="64" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="64" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="80" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="380" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>1</v>
       </c>
@@ -1472,21 +1725,33 @@
         <v>2</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="80" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="380" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="80" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="80" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>3</v>
       </c>
@@ -1494,43 +1759,55 @@
         <v>4</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="80" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="80" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C46" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="80" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
         <v>86</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="80" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="80" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="80" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="80" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="80" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>6</v>
       </c>
@@ -1538,32 +1815,41 @@
         <v>4</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="80" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="80" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="80" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="80" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="80" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="80" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>7</v>
       </c>
@@ -1571,303 +1857,383 @@
         <v>8</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="80" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="80" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C53" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" ht="48" x14ac:dyDescent="0.2">
-      <c r="A54" s="1" t="s">
+      <c r="C54" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="320" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="B55" s="1" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" ht="96" x14ac:dyDescent="0.2">
-      <c r="A55" s="1" t="s">
+      <c r="C55" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B56" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C55" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A56" s="1" t="s">
+      <c r="C56" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="112" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B57" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C56" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="80" x14ac:dyDescent="0.2">
-      <c r="A57" s="1" t="s">
+      <c r="C57" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="112" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B58" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="C58" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B59" s="1" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" ht="64" x14ac:dyDescent="0.2">
-      <c r="A58" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" ht="64" x14ac:dyDescent="0.2">
-      <c r="A59" s="1" t="s">
+      <c r="C59" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="D59" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="144" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="C60" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" ht="144" x14ac:dyDescent="0.2">
-      <c r="A60" s="1" t="s">
+      <c r="C61" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="D61" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="96" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="B62" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="80" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" ht="48" x14ac:dyDescent="0.2">
-      <c r="A61" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" ht="96" x14ac:dyDescent="0.2">
-      <c r="A62" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" ht="64" x14ac:dyDescent="0.2">
-      <c r="A63" s="1" t="s">
+      <c r="C68" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="A69" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B63" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" ht="80" x14ac:dyDescent="0.2">
-      <c r="A64" s="1" t="s">
+      <c r="B72" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B64" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" ht="48" x14ac:dyDescent="0.2">
-      <c r="A65" s="1" t="s">
+      <c r="C72" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B65" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A66" s="1" t="s">
+      <c r="B73" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B66" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" ht="48" x14ac:dyDescent="0.2">
-      <c r="A67" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" ht="48" x14ac:dyDescent="0.2">
-      <c r="A68" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C68" s="2" t="s">
+      <c r="C73" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C74" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="64" x14ac:dyDescent="0.2">
-      <c r="A69" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C69" s="2" t="s">
+    <row r="75" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B75" s="1" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" ht="48" x14ac:dyDescent="0.2">
-      <c r="A70" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C70" s="2" t="s">
+      <c r="C75" s="1" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" ht="48" x14ac:dyDescent="0.2">
-      <c r="A71" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C71" s="2" t="s">
+      <c r="D75" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B76" s="1" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A72" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C72" s="2" t="s">
+      <c r="C76" s="1" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" ht="48" x14ac:dyDescent="0.2">
-      <c r="A73" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C73" s="2" t="s">
+      <c r="D76" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B77" s="1" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" ht="48" x14ac:dyDescent="0.2">
-      <c r="A74" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C74" s="1" t="s">
+      <c r="C77" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A75" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A76" s="1" t="s">
+      <c r="B78" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B76" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A77" s="1" t="s">
+      <c r="B79" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A80" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B77" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A78" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A79" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A80" s="1" t="s">
-        <v>133</v>
-      </c>
       <c r="B80" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E9" r:id="rId1" xr:uid="{822A0BDC-AF56-B148-B1E6-28E798DCA458}"/>
+    <hyperlink ref="E10" r:id="rId2" xr:uid="{FDBD3818-9066-A04B-B91F-D5DABAD585E2}"/>
+    <hyperlink ref="E11" r:id="rId3" xr:uid="{CD714593-047E-C041-AD81-A493D0502513}"/>
+    <hyperlink ref="E13" r:id="rId4" xr:uid="{1A35EBF3-75BF-5044-BA0C-7E93BB212DF9}"/>
+    <hyperlink ref="E16" r:id="rId5" location=":~:text=The%20ADA%20defines%20a%20person,not%20currently%20have%20a%20disability." display="https://adata.org/faq/what-definition-disability-under-ada - :~:text=The%20ADA%20defines%20a%20person,not%20currently%20have%20a%20disability." xr:uid="{0C38394D-51D1-2248-8539-3FAE47C21C32}"/>
+    <hyperlink ref="E26" r:id="rId6" xr:uid="{1B3A5719-54CD-DD47-BAB4-4B14D68D2D1B}"/>
+    <hyperlink ref="E27" r:id="rId7" xr:uid="{FC65F9B2-DC27-324B-BB24-996C51CF5D6A}"/>
+    <hyperlink ref="E28" r:id="rId8" xr:uid="{63837D77-2D06-6349-B5FD-33D2534A9481}"/>
+    <hyperlink ref="E29" r:id="rId9" xr:uid="{56FCD263-678C-674F-B4A5-1A2F2C1B907C}"/>
+    <hyperlink ref="E43" r:id="rId10" xr:uid="{699CC563-4F69-EB40-8216-E4FE014623A6}"/>
+    <hyperlink ref="E44" r:id="rId11" xr:uid="{0A582372-2B28-B843-8CE5-868EBC57C6A1}"/>
+    <hyperlink ref="E55" r:id="rId12" location=":~:text=We%20ask%20questions%20about%20the,assistance%20for%20populations%20in%20need." display="https://www.census.gov/acs/www/about/why-we-ask-each-question/income/ - :~:text=We%20ask%20questions%20about%20the,assistance%20for%20populations%20in%20need." xr:uid="{821723F2-F703-B74D-AAFA-0E80CC12BA2D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add text to historical and update baseline sources.
</commit_message>
<xml_diff>
--- a/Data/Baseline.xlsx
+++ b/Data/Baseline.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abautist/Dropbox (University of Oregon)/Rapid Response Research (R3)/Data Management R3/EE_R3 Question Bank/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akunerth/Dropbox (University of Oregon)/Rapid Response Research (R3)/Data Management R3/EE_R3 Question Bank/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3506F8B4-6029-C640-841A-C8D7D845B660}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC748062-E040-A949-8181-F78090B216E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40460" yWindow="900" windowWidth="20600" windowHeight="15580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="194">
   <si>
     <t xml:space="preserve">• Not at all _x000D_
 • Several days _x000D_
@@ -865,6 +865,9 @@
 •	No, and I DO NOT expect to receive a federal stimulus check
 •	Unsure if I will receive a federal stimulus check
 •	Other</t>
+  </si>
+  <si>
+    <t>RAPID Team Modified from National Compensation Survey</t>
   </si>
 </sst>
 </file>
@@ -1247,8 +1250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="D89" sqref="D89:D94"/>
+    <sheetView tabSelected="1" topLeftCell="A92" zoomScale="125" workbookViewId="0">
+      <selection activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2073,6 +2076,9 @@
       <c r="C57" s="2" t="s">
         <v>93</v>
       </c>
+      <c r="D57" s="1" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="58" spans="1:5" ht="64" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
@@ -2084,6 +2090,9 @@
       <c r="C58" s="2" t="s">
         <v>93</v>
       </c>
+      <c r="D58" s="1" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="59" spans="1:5" ht="64" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
@@ -2095,6 +2104,9 @@
       <c r="C59" s="2" t="s">
         <v>93</v>
       </c>
+      <c r="D59" s="1" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="60" spans="1:5" ht="128" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
@@ -2106,6 +2118,9 @@
       <c r="C60" s="2" t="s">
         <v>93</v>
       </c>
+      <c r="D60" s="1" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="61" spans="1:5" ht="128" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
@@ -2117,6 +2132,9 @@
       <c r="C61" s="2" t="s">
         <v>93</v>
       </c>
+      <c r="D61" s="1" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="62" spans="1:5" ht="64" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
@@ -2128,6 +2146,9 @@
       <c r="C62" s="2" t="s">
         <v>93</v>
       </c>
+      <c r="D62" s="1" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="63" spans="1:5" ht="64" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
@@ -2139,6 +2160,9 @@
       <c r="C63" s="2" t="s">
         <v>93</v>
       </c>
+      <c r="D63" s="1" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="64" spans="1:5" ht="160" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
@@ -2150,6 +2174,9 @@
       <c r="C64" s="2" t="s">
         <v>93</v>
       </c>
+      <c r="D64" s="1" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="65" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
@@ -2161,8 +2188,11 @@
       <c r="C65" s="2" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="D65" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="96" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>175</v>
       </c>
@@ -2171,6 +2201,9 @@
       </c>
       <c r="C66" s="2" t="s">
         <v>93</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="96" x14ac:dyDescent="0.2">
@@ -2183,6 +2216,9 @@
       <c r="C67" s="2" t="s">
         <v>93</v>
       </c>
+      <c r="D67" s="1" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="68" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
@@ -2194,6 +2230,9 @@
       <c r="C68" s="2" t="s">
         <v>93</v>
       </c>
+      <c r="D68" s="1" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="69" spans="1:4" ht="192" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
@@ -2205,6 +2244,9 @@
       <c r="C69" s="2" t="s">
         <v>93</v>
       </c>
+      <c r="D69" s="1" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="70" spans="1:4" ht="96" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
@@ -2215,6 +2257,9 @@
       </c>
       <c r="C70" s="2" t="s">
         <v>93</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="112" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Updated home text, baseline and followup
</commit_message>
<xml_diff>
--- a/Data/Baseline.xlsx
+++ b/Data/Baseline.xlsx
@@ -5,22 +5,22 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akunerth/Dropbox (University of Oregon)/Rapid Response Research (R3)/Data Management R3/EE_R3 Question Bank/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abautist/Dropbox (University of Oregon)/Rapid Response Research (R3)/Data Management R3/EE_R3 Question Bank/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC748062-E040-A949-8181-F78090B216E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1500C820-24FD-1A4A-88D6-F9AABB414BFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028" concurrentCalc="0"/>
+  <calcPr calcId="191028"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="197">
   <si>
     <t xml:space="preserve">• Not at all _x000D_
 • Several days _x000D_
@@ -868,6 +868,19 @@
   </si>
   <si>
     <t>RAPID Team Modified from National Compensation Survey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What was your partner's employment status prior to the coronavirus (COVID-19) Pandemic? If you do not have a partner, please select not applicable. </t>
+  </si>
+  <si>
+    <t>• Working
+• Unemployed or laid off
+• Temporarily out of work or furloughed
+• Other
+• Not applicable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is your partner's current employment status? If you do not have a partner, please select not applicable. </t>
   </si>
 </sst>
 </file>
@@ -1248,10 +1261,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E94"/>
+  <dimension ref="A1:E96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D69" sqref="D69"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="125" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2222,133 +2235,133 @@
     </row>
     <row r="68" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>178</v>
+        <v>194</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>93</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" ht="192" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>181</v>
+        <v>195</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>93</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" ht="96" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>93</v>
       </c>
       <c r="D70" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="192" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D71" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="112" x14ac:dyDescent="0.2">
-      <c r="A71" s="1" t="s">
+    <row r="72" spans="1:4" ht="96" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="112" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B73" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C71" s="2" t="s">
+      <c r="C73" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D71" s="1" t="s">
+      <c r="D73" s="1" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="112" x14ac:dyDescent="0.2">
-      <c r="A72" s="1" t="s">
+    <row r="74" spans="1:4" ht="112" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="B74" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C72" s="2" t="s">
+      <c r="C74" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D72" s="1" t="s">
+      <c r="D74" s="1" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A73" s="1" t="s">
+    <row r="75" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B73" s="1" t="s">
+      <c r="B75" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C73" s="2" t="s">
+      <c r="C75" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="D73" s="1" t="s">
+      <c r="D75" s="1" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="144" x14ac:dyDescent="0.2">
-      <c r="A74" s="1" t="s">
+    <row r="76" spans="1:4" ht="144" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="B76" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C74" s="2" t="s">
+      <c r="C76" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="D74" s="1" t="s">
+      <c r="D76" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A75" s="1" t="s">
+    <row r="77" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" ht="96" x14ac:dyDescent="0.2">
-      <c r="A76" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A77" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>110</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>108</v>
@@ -2357,9 +2370,9 @@
         <v>164</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4" ht="96" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>110</v>
@@ -2371,9 +2384,9 @@
         <v>164</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>110</v>
@@ -2385,133 +2398,133 @@
         <v>164</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>108</v>
       </c>
+      <c r="D80" s="1" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="81" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="D81" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>107</v>
+        <v>114</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>115</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>117</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="D84" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    </row>
+    <row r="85" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="D85" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    </row>
+    <row r="86" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="C86" s="2" t="s">
         <v>122</v>
       </c>
+      <c r="D86" s="1" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="87" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="C87" s="2" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="D87" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="A89" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="A90" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A89" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D89" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A90" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>125</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="D90" s="1" t="s">
-        <v>152</v>
-      </c>
     </row>
     <row r="91" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>125</v>
@@ -2525,7 +2538,7 @@
     </row>
     <row r="92" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>125</v>
@@ -2539,7 +2552,7 @@
     </row>
     <row r="93" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>125</v>
@@ -2553,15 +2566,43 @@
     </row>
     <row r="94" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>165</v>
+        <v>128</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>69</v>
+        <v>125</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>125</v>
       </c>
       <c r="D94" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A95" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A96" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D96" s="1" t="s">
         <v>152</v>
       </c>
     </row>

</xml_diff>